<commit_message>
Added data folder including example files
</commit_message>
<xml_diff>
--- a/data/02_intermediate/svn_df_clean.xlsx
+++ b/data/02_intermediate/svn_df_clean.xlsx
@@ -2656,17 +2656,17 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '110283', 'branchesdevelop', 'line', 'revis', '283', 'test', 'version']</t>
+          <t>['creat', 'tag', '110283', 'branchesanonymisedpath', 'test', 'version']</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '110283'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '283'], ['283', 'test'], ['test', 'version']]</t>
+          <t>[['creat', 'tag'], ['tag', '110283'], ['branchesanonymisedpath', 'test'], ['test', 'version']]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '110283'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '283'], ['revis', '283', 'test'], ['283', 'test', 'version']]</t>
+          <t>[['creat', 'tag', '110283'], ['branchesanonymisedpath', 'test', 'version']]</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -2762,17 +2762,17 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '110287', 'branchesdevelop', 'line', 'revis', '287', 'test', 'version', '2519', '2579']</t>
+          <t>['creat', 'tag', '110287', 'branchesanonymisedpath', 'test', 'version', '2519', '2579']</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '110287'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '287'], ['287', 'test'], ['test', 'version'], ['version', '2519']]</t>
+          <t>[['creat', 'tag'], ['tag', '110287'], ['branchesanonymisedpath', 'test'], ['test', 'version'], ['version', '2519']]</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '110287'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '287'], ['revis', '287', 'test'], ['287', 'test', 'version'], ['test', 'version', '2519']]</t>
+          <t>[['creat', 'tag', '110287'], ['branchesanonymisedpath', 'test', 'version'], ['test', 'version', '2519']]</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -5249,17 +5249,17 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140399', 'branchesdevelop', 'line', 'revis', '399']</t>
+          <t>['creat', 'tag', '140399', 'branchesanonymisedpath']</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140399'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '399']]</t>
+          <t>[['creat', 'tag'], ['tag', '140399']]</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140399'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '399']]</t>
+          <t>[['creat', 'tag', '140399']]</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
@@ -5875,17 +5875,17 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140410', 'branchesdevelop', 'line', 'revis', '410']</t>
+          <t>['creat', 'tag', '140410', 'branchesanonymisedpath']</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140410'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '410']]</t>
+          <t>[['creat', 'tag'], ['tag', '140410']]</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140410'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '410']]</t>
+          <t>[['creat', 'tag', '140410']]</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -5981,17 +5981,17 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140414', 'branchesdevelop', 'line', 'revis', '414']</t>
+          <t>['creat', 'tag', '140414', 'branchesanonymisedpath']</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140414'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '414']]</t>
+          <t>[['creat', 'tag'], ['tag', '140414']]</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140414'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '414']]</t>
+          <t>[['creat', 'tag', '140414']]</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
@@ -6607,17 +6607,17 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140448', 'branchesdevelop', 'line', 'revis', '448']</t>
+          <t>['creat', 'tag', '140448', 'branchesanonymisedpath']</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140448'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '448']]</t>
+          <t>[['creat', 'tag'], ['tag', '140448']]</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140448'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '448']]</t>
+          <t>[['creat', 'tag', '140448']]</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
@@ -6908,17 +6908,17 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140458', 'branchesdevelop', 'line', 'revis', '458', 'test']</t>
+          <t>['creat', 'tag', '140458', 'branchesanonymisedpath', 'test']</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140458'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '458'], ['458', 'test']]</t>
+          <t>[['creat', 'tag'], ['tag', '140458'], ['branchesanonymisedpath', 'test']]</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140458'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '458'], ['revis', '458', 'test']]</t>
+          <t>[['creat', 'tag', '140458']]</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -7079,17 +7079,17 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140461', 'branchesdevelop', 'line', 'revis', '461']</t>
+          <t>['creat', 'tag', '140461', 'branchesanonymisedpath']</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140461'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '461']]</t>
+          <t>[['creat', 'tag'], ['tag', '140461']]</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140461'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '461']]</t>
+          <t>[['creat', 'tag', '140461']]</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -9104,17 +9104,17 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140525', 'branchesdevelop', 'line', 'revis', '525', 'test']</t>
+          <t>['creat', 'tag', '140525', 'branchesanonymisedpath', 'test']</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140525'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '525'], ['525', 'test']]</t>
+          <t>[['creat', 'tag'], ['tag', '140525'], ['branchesanonymisedpath', 'test']]</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140525'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '525'], ['revis', '525', 'test']]</t>
+          <t>[['creat', 'tag', '140525']]</t>
         </is>
       </c>
       <c r="H141" t="inlineStr"/>
@@ -9405,17 +9405,17 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140535', 'branchesdevelop', 'line', 'revis', '535', 'test']</t>
+          <t>['creat', 'tag', '140535', 'branchesanonymisedpath', 'test']</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140535'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '535'], ['535', 'test']]</t>
+          <t>[['creat', 'tag'], ['tag', '140535'], ['branchesanonymisedpath', 'test']]</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140535'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '535'], ['revis', '535', 'test']]</t>
+          <t>[['creat', 'tag', '140535']]</t>
         </is>
       </c>
       <c r="H146" t="inlineStr"/>
@@ -9511,17 +9511,17 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>['creat', 'tag', '140537', 'branchesdevelop', 'line', 'revis', '537', 'test']</t>
+          <t>['creat', 'tag', '140537', 'branchesanonymisedpath', 'test']</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>[['creat', 'tag'], ['tag', '140537'], ['branchesdevelop', 'line'], ['line', 'revis'], ['revis', '537'], ['537', 'test']]</t>
+          <t>[['creat', 'tag'], ['tag', '140537'], ['branchesanonymisedpath', 'test']]</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>[['creat', 'tag', '140537'], ['branchesdevelop', 'line', 'revis'], ['line', 'revis', '537'], ['revis', '537', 'test']]</t>
+          <t>[['creat', 'tag', '140537']]</t>
         </is>
       </c>
       <c r="H148" t="inlineStr"/>

</xml_diff>